<commit_message>
Updating attendance files 4th march
</commit_message>
<xml_diff>
--- a/attendance-files/FA-II/FA-II (B) Attendance Sheet.xlsx
+++ b/attendance-files/FA-II/FA-II (B) Attendance Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="171">
   <si>
     <t>Indian Institute of Management Indore</t>
   </si>
@@ -1620,7 +1620,7 @@
       </c>
       <c r="E7" s="26">
         <f t="shared" ref="E7:E95" si="1">IF(D7&gt;0,COUNTIF(G7:Z7,"A"),"")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="27">
         <f t="shared" ref="F7:F95" si="2">IF(D7&gt;0,COUNTIF(G7:Z7,"P"),"")</f>
@@ -1647,7 +1647,9 @@
       </c>
       <c r="T7" s="30"/>
       <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
+      <c r="V7" s="29" t="s">
+        <v>22</v>
+      </c>
       <c r="W7" s="30"/>
       <c r="X7" s="30"/>
       <c r="Y7" s="30"/>
@@ -1758,7 +1760,7 @@
       </c>
       <c r="E10" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="34">
         <f t="shared" si="2"/>
@@ -1780,7 +1782,9 @@
       <c r="T10" s="36"/>
       <c r="U10" s="36"/>
       <c r="V10" s="36"/>
-      <c r="W10" s="36"/>
+      <c r="W10" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X10" s="36"/>
       <c r="Y10" s="36"/>
       <c r="Z10" s="36"/>
@@ -1802,7 +1806,7 @@
       </c>
       <c r="E11" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="34">
         <f t="shared" si="2"/>
@@ -1824,7 +1828,9 @@
       <c r="T11" s="36"/>
       <c r="U11" s="36"/>
       <c r="V11" s="36"/>
-      <c r="W11" s="36"/>
+      <c r="W11" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X11" s="36"/>
       <c r="Y11" s="36"/>
       <c r="Z11" s="36"/>
@@ -1892,7 +1898,7 @@
       </c>
       <c r="E13" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="34">
         <f t="shared" si="2"/>
@@ -1918,7 +1924,9 @@
       <c r="T13" s="36"/>
       <c r="U13" s="36"/>
       <c r="V13" s="36"/>
-      <c r="W13" s="36"/>
+      <c r="W13" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X13" s="36"/>
       <c r="Y13" s="36"/>
       <c r="Z13" s="36"/>
@@ -1940,7 +1948,7 @@
       </c>
       <c r="E14" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="34">
         <f t="shared" si="2"/>
@@ -1961,7 +1969,9 @@
       <c r="S14" s="36"/>
       <c r="T14" s="36"/>
       <c r="U14" s="36"/>
-      <c r="V14" s="36"/>
+      <c r="V14" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="W14" s="36"/>
       <c r="X14" s="36"/>
       <c r="Y14" s="36"/>
@@ -1984,7 +1994,7 @@
       </c>
       <c r="E15" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="34">
         <f t="shared" si="2"/>
@@ -2012,7 +2022,9 @@
       <c r="T15" s="36"/>
       <c r="U15" s="36"/>
       <c r="V15" s="36"/>
-      <c r="W15" s="36"/>
+      <c r="W15" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X15" s="36"/>
       <c r="Y15" s="36"/>
       <c r="Z15" s="36"/>
@@ -2078,7 +2090,7 @@
       </c>
       <c r="E17" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F17" s="34">
         <f t="shared" si="2"/>
@@ -2107,8 +2119,12 @@
       <c r="S17" s="36"/>
       <c r="T17" s="36"/>
       <c r="U17" s="36"/>
-      <c r="V17" s="36"/>
-      <c r="W17" s="36"/>
+      <c r="V17" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="W17" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X17" s="36"/>
       <c r="Y17" s="36"/>
       <c r="Z17" s="36"/>
@@ -2176,7 +2192,7 @@
       </c>
       <c r="E19" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" s="34">
         <f t="shared" si="2"/>
@@ -2204,7 +2220,9 @@
       <c r="T19" s="36"/>
       <c r="U19" s="36"/>
       <c r="V19" s="36"/>
-      <c r="W19" s="36"/>
+      <c r="W19" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X19" s="36"/>
       <c r="Y19" s="36"/>
       <c r="Z19" s="36"/>
@@ -2478,7 +2496,7 @@
       </c>
       <c r="E25" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F25" s="34">
         <f t="shared" si="2"/>
@@ -2508,7 +2526,9 @@
       </c>
       <c r="U25" s="36"/>
       <c r="V25" s="36"/>
-      <c r="W25" s="36"/>
+      <c r="W25" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X25" s="36"/>
       <c r="Y25" s="36"/>
       <c r="Z25" s="36"/>
@@ -2530,7 +2550,7 @@
       </c>
       <c r="E26" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F26" s="34">
         <f t="shared" si="2"/>
@@ -2559,7 +2579,9 @@
       <c r="U26" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="V26" s="36"/>
+      <c r="V26" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="W26" s="36"/>
       <c r="X26" s="36"/>
       <c r="Y26" s="36"/>
@@ -2632,7 +2654,7 @@
       </c>
       <c r="E28" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F28" s="34">
         <f t="shared" si="2"/>
@@ -2658,7 +2680,9 @@
       <c r="T28" s="36"/>
       <c r="U28" s="36"/>
       <c r="V28" s="36"/>
-      <c r="W28" s="36"/>
+      <c r="W28" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X28" s="36"/>
       <c r="Y28" s="36"/>
       <c r="Z28" s="36"/>
@@ -2680,7 +2704,7 @@
       </c>
       <c r="E29" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" s="34">
         <f t="shared" si="2"/>
@@ -2704,7 +2728,9 @@
       <c r="T29" s="36"/>
       <c r="U29" s="36"/>
       <c r="V29" s="36"/>
-      <c r="W29" s="36"/>
+      <c r="W29" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X29" s="36"/>
       <c r="Y29" s="36"/>
       <c r="Z29" s="36"/>
@@ -2818,7 +2844,7 @@
       </c>
       <c r="E32" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" s="34">
         <f t="shared" si="2"/>
@@ -2845,7 +2871,9 @@
       <c r="U32" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="V32" s="36"/>
+      <c r="V32" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="W32" s="36"/>
       <c r="X32" s="36"/>
       <c r="Y32" s="36"/>
@@ -2868,7 +2896,7 @@
       </c>
       <c r="E33" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F33" s="34">
         <f t="shared" si="2"/>
@@ -2894,7 +2922,9 @@
       <c r="T33" s="36"/>
       <c r="U33" s="36"/>
       <c r="V33" s="36"/>
-      <c r="W33" s="36"/>
+      <c r="W33" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X33" s="36"/>
       <c r="Y33" s="36"/>
       <c r="Z33" s="36"/>
@@ -2916,7 +2946,7 @@
       </c>
       <c r="E34" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F34" s="34">
         <f t="shared" si="2"/>
@@ -2940,7 +2970,9 @@
       </c>
       <c r="U34" s="36"/>
       <c r="V34" s="36"/>
-      <c r="W34" s="36"/>
+      <c r="W34" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X34" s="36"/>
       <c r="Y34" s="36"/>
       <c r="Z34" s="36"/>
@@ -3012,7 +3044,7 @@
       </c>
       <c r="E36" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F36" s="34">
         <f t="shared" si="2"/>
@@ -3038,7 +3070,9 @@
       </c>
       <c r="U36" s="36"/>
       <c r="V36" s="36"/>
-      <c r="W36" s="36"/>
+      <c r="W36" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X36" s="36"/>
       <c r="Y36" s="36"/>
       <c r="Z36" s="36"/>
@@ -3060,7 +3094,7 @@
       </c>
       <c r="E37" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F37" s="34">
         <f t="shared" si="2"/>
@@ -3091,7 +3125,9 @@
       <c r="U37" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="V37" s="36"/>
+      <c r="V37" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="W37" s="36"/>
       <c r="X37" s="36"/>
       <c r="Y37" s="36"/>
@@ -3114,7 +3150,7 @@
       </c>
       <c r="E38" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F38" s="34">
         <f t="shared" si="2"/>
@@ -3140,7 +3176,9 @@
         <v>22</v>
       </c>
       <c r="V38" s="36"/>
-      <c r="W38" s="36"/>
+      <c r="W38" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X38" s="36"/>
       <c r="Y38" s="36"/>
       <c r="Z38" s="36"/>
@@ -3162,7 +3200,7 @@
       </c>
       <c r="E39" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F39" s="34">
         <f t="shared" si="2"/>
@@ -3192,7 +3230,9 @@
       <c r="T39" s="36"/>
       <c r="U39" s="36"/>
       <c r="V39" s="36"/>
-      <c r="W39" s="36"/>
+      <c r="W39" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X39" s="36"/>
       <c r="Y39" s="36"/>
       <c r="Z39" s="36"/>
@@ -3258,7 +3298,7 @@
       </c>
       <c r="E41" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F41" s="34">
         <f t="shared" si="2"/>
@@ -3286,7 +3326,9 @@
       </c>
       <c r="U41" s="36"/>
       <c r="V41" s="36"/>
-      <c r="W41" s="36"/>
+      <c r="W41" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X41" s="36"/>
       <c r="Y41" s="36"/>
       <c r="Z41" s="36"/>
@@ -3308,7 +3350,7 @@
       </c>
       <c r="E42" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F42" s="34">
         <f t="shared" si="2"/>
@@ -3332,7 +3374,9 @@
       <c r="T42" s="36"/>
       <c r="U42" s="36"/>
       <c r="V42" s="36"/>
-      <c r="W42" s="36"/>
+      <c r="W42" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X42" s="36"/>
       <c r="Y42" s="36"/>
       <c r="Z42" s="36"/>
@@ -3744,7 +3788,7 @@
       </c>
       <c r="E51" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F51" s="34">
         <f t="shared" si="2"/>
@@ -3769,7 +3813,9 @@
       <c r="S51" s="36"/>
       <c r="T51" s="36"/>
       <c r="U51" s="36"/>
-      <c r="V51" s="36"/>
+      <c r="V51" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="W51" s="36"/>
       <c r="X51" s="36"/>
       <c r="Y51" s="36"/>
@@ -3890,7 +3936,7 @@
       </c>
       <c r="E54" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F54" s="34">
         <f t="shared" si="2"/>
@@ -3916,7 +3962,9 @@
       <c r="T54" s="36"/>
       <c r="U54" s="36"/>
       <c r="V54" s="36"/>
-      <c r="W54" s="36"/>
+      <c r="W54" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X54" s="36"/>
       <c r="Y54" s="36"/>
       <c r="Z54" s="36"/>
@@ -4180,7 +4228,7 @@
       </c>
       <c r="E60" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F60" s="34">
         <f t="shared" si="2"/>
@@ -4206,7 +4254,9 @@
       <c r="T60" s="36"/>
       <c r="U60" s="36"/>
       <c r="V60" s="36"/>
-      <c r="W60" s="36"/>
+      <c r="W60" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X60" s="36"/>
       <c r="Y60" s="36"/>
       <c r="Z60" s="36"/>
@@ -4370,7 +4420,7 @@
       </c>
       <c r="E64" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F64" s="34">
         <f t="shared" si="2"/>
@@ -4394,7 +4444,9 @@
       <c r="T64" s="36"/>
       <c r="U64" s="36"/>
       <c r="V64" s="36"/>
-      <c r="W64" s="36"/>
+      <c r="W64" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X64" s="36"/>
       <c r="Y64" s="36"/>
       <c r="Z64" s="36"/>
@@ -4700,7 +4752,7 @@
       </c>
       <c r="E71" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F71" s="34">
         <f t="shared" si="2"/>
@@ -4722,7 +4774,9 @@
       <c r="T71" s="36"/>
       <c r="U71" s="36"/>
       <c r="V71" s="36"/>
-      <c r="W71" s="36"/>
+      <c r="W71" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="X71" s="36"/>
       <c r="Y71" s="36"/>
       <c r="Z71" s="36"/>
@@ -5040,7 +5094,7 @@
       </c>
       <c r="E78" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F78" s="34">
         <f t="shared" si="2"/>
@@ -5063,7 +5117,9 @@
       <c r="S78" s="36"/>
       <c r="T78" s="36"/>
       <c r="U78" s="36"/>
-      <c r="V78" s="36"/>
+      <c r="V78" s="38" t="s">
+        <v>22</v>
+      </c>
       <c r="W78" s="36"/>
       <c r="X78" s="36"/>
       <c r="Y78" s="36"/>

</xml_diff>